<commit_message>
just getting version up to date
</commit_message>
<xml_diff>
--- a/Data/modified_parameters_scenario_3/population_scenario_high_growth.xlsx
+++ b/Data/modified_parameters_scenario_3/population_scenario_high_growth.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/954e9104582efe7e/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/954e9104582efe7e/Documents/Python/TEP4290_project/data/modified_parameters_scenario_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{CAF32350-8AAE-40A9-85F4-445FF36C4017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -438,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BBC161-BDCA-49EC-9211-998BEFF6025D}">
   <dimension ref="A1:B452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A419" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A438" workbookViewId="0">
       <selection activeCell="D419" sqref="D419"/>
     </sheetView>
   </sheetViews>

</xml_diff>